<commit_message>
Orginfo, Excel einlesen, Flask bestandteil von Main
</commit_message>
<xml_diff>
--- a/excelpkg/Kunden-Excel-DRAFT.xlsx
+++ b/excelpkg/Kunden-Excel-DRAFT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Documents\WebexCallingProv\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/630c9287b3bb8d93/03_Techniker Schule/Techniker Arbeit/WebexCallingProv/excelpkg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E292E0D-B373-416E-ABF7-3B55EED93FF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{2E292E0D-B373-416E-ABF7-3B55EED93FF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7BCE92EC-9389-5C4B-B691-E76AB2E0FE48}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3506BBAA-2EB0-3649-9FB5-A30459E31741}"/>
+    <workbookView xWindow="42340" yWindow="-540" windowWidth="29040" windowHeight="16000" xr2:uid="{3506BBAA-2EB0-3649-9FB5-A30459E31741}"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>+497117828355</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -443,21 +446,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3540F1-6548-7943-9FC4-7B110902D3A7}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
-    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +489,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -513,6 +516,51 @@
       </c>
       <c r="I2">
         <v>8851</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -531,32 +579,32 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>8841</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>8851</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>8845</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>8865</v>
       </c>

</xml_diff>